<commit_message>
qPCR Adjustment in R with comments
</commit_message>
<xml_diff>
--- a/qPCR/adjustment/Neill2018calibrationsAdjusted.xlsx
+++ b/qPCR/adjustment/Neill2018calibrationsAdjusted.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbyrd/StapletonLab/Stapleton_Lab/qPCR/adjustment/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0275383A-9E4A-B044-BE81-90A1ECCA244F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12210" tabRatio="500"/>
+    <workbookView xWindow="400" yWindow="840" windowWidth="40160" windowHeight="24360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>amount_gblock+ire</t>
   </si>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1094,452 +1095,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>unif_applied</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.20068738765808514"/>
-                  <c:y val="-0.42626123542216815"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$2:$I$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>18.400666666666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.360666666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18.380666666666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22.060666666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22.230666666666668</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>21.940666666666669</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25.520666666666667</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25.510666666666669</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>25.360666666666667</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28.740666666666666</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>28.750666666666667</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>28.660666666666668</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>31.640666666666668</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>31.610666666666667</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>31.630666666666666</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F9F6-4E31-B732-2C8AF0B7A7AD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="672271696"/>
-        <c:axId val="672272024"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="672271696"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="672272024"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="672272024"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="672271696"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1690,7 +1246,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$32</c:f>
+              <c:f>Sheet1!$H$2:$H$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -1704,40 +1260,40 @@
                   <c:v>18.849999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.529999999999998</c:v>
+                  <c:v>22.373333333333331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.7</c:v>
+                  <c:v>22.543333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.41</c:v>
+                  <c:v>22.253333333333334</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.86333333333333</c:v>
+                  <c:v>25.553333333333331</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.853333333333332</c:v>
+                  <c:v>25.543333333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25.70333333333333</c:v>
+                  <c:v>25.393333333333331</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.053333333333331</c:v>
+                  <c:v>28.39</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29.063333333333333</c:v>
+                  <c:v>28.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.973333333333333</c:v>
+                  <c:v>28.310000000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31.816666666666666</c:v>
+                  <c:v>31.176666666666666</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>31.786666666666665</c:v>
+                  <c:v>31.146666666666665</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.806666666666665</c:v>
+                  <c:v>31.166666666666664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1929,7 +1485,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1984,7 +1540,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$1</c:f>
+              <c:f>Sheet1!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2081,7 +1637,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$32</c:f>
+              <c:f>Sheet1!$K$2:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -2135,7 +1691,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$32</c:f>
+              <c:f>Sheet1!$N$2:$N$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -2374,7 +1930,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2429,7 +1985,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$1</c:f>
+              <c:f>Sheet1!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2526,7 +2082,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$32</c:f>
+              <c:f>Sheet1!$K$2:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -2580,7 +2136,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$32</c:f>
+              <c:f>Sheet1!$M$2:$M$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -2819,7 +2375,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2874,7 +2430,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$1</c:f>
+              <c:f>Sheet1!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2957,7 +2513,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$32</c:f>
+              <c:f>Sheet1!$K$2:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -3011,7 +2567,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$2:$S$32</c:f>
+              <c:f>Sheet1!$Q$2:$Q$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -3250,7 +2806,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3305,7 +2861,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$1</c:f>
+              <c:f>Sheet1!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3388,7 +2944,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$32</c:f>
+              <c:f>Sheet1!$K$2:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -3442,7 +2998,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$32</c:f>
+              <c:f>Sheet1!$R$2:$R$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -3961,46 +3517,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7098,522 +6614,6 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8176,7 +7176,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -8206,22 +7206,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>804862</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>173267</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>34570</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1181100</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>719980</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>100065</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10">
+        <xdr:cNvPr id="12" name="Chart 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CFA8361-6E10-47D2-B984-6341D059742E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88AF8FCB-C768-4C7B-9746-33441D22FDEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8241,49 +7241,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>661987</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88AF8FCB-C768-4C7B-9746-33441D22FDEC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>847725</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -8305,7 +7269,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8313,13 +7277,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -8341,7 +7305,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8349,13 +7313,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -8377,7 +7341,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8385,13 +7349,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1090612</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -8413,7 +7377,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8684,28 +7648,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -8725,48 +7688,42 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <f>LOG10(C2)</f>
+        <f t="shared" ref="B2:B16" si="0">LOG10(C2)</f>
         <v>2</v>
       </c>
       <c r="C2">
@@ -8782,53 +7739,46 @@
         <v>18.73</v>
       </c>
       <c r="G2">
-        <v>0.66066666666666696</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H2">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="I2">
         <f>D2+G2</f>
-        <v>18.400666666666666</v>
-      </c>
-      <c r="J2">
-        <f>D2+H2</f>
         <v>18.869999999999997</v>
       </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K16" si="1">LOG10(L2)</f>
+        <v>2.3010299956639813</v>
+      </c>
+      <c r="L2">
+        <v>200</v>
+      </c>
       <c r="M2">
-        <f>LOG10(N2)</f>
-        <v>2.3010299956639813</v>
+        <v>16.46</v>
       </c>
       <c r="N2">
-        <v>200</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="O2">
-        <v>16.46</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P2">
-        <v>17.899999999999999</v>
+        <v>1.5533333333333299</v>
       </c>
       <c r="Q2">
-        <v>1.1966666666666601</v>
+        <f t="shared" ref="Q2:Q16" si="2">M2+O2</f>
+        <v>17.656666666666659</v>
       </c>
       <c r="R2">
-        <v>1.5533333333333299</v>
-      </c>
-      <c r="S2">
-        <f>O2+Q2</f>
-        <v>17.656666666666659</v>
-      </c>
-      <c r="T2">
-        <f>O2+R2</f>
+        <f t="shared" ref="R2:R16" si="3">M2+P2</f>
         <v>18.013333333333332</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <f>LOG10(C3)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C3">
@@ -8844,53 +7794,46 @@
         <v>18.940000000000001</v>
       </c>
       <c r="G3">
-        <v>0.66066666666666696</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H3">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="I3">
         <f>D3+G3</f>
-        <v>18.360666666666667</v>
-      </c>
-      <c r="J3">
-        <f>D3+H3</f>
         <v>18.829999999999998</v>
       </c>
+      <c r="K3">
+        <f t="shared" si="1"/>
+        <v>2.3010299956639813</v>
+      </c>
+      <c r="L3">
+        <v>200</v>
+      </c>
       <c r="M3">
-        <f>LOG10(N3)</f>
-        <v>2.3010299956639813</v>
+        <v>16.420000000000002</v>
       </c>
       <c r="N3">
-        <v>200</v>
+        <v>18.03</v>
       </c>
       <c r="O3">
-        <v>16.420000000000002</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P3">
-        <v>18.03</v>
+        <v>1.5533333333333299</v>
       </c>
       <c r="Q3">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>17.61666666666666</v>
       </c>
       <c r="R3">
-        <v>1.5533333333333299</v>
-      </c>
-      <c r="S3">
-        <f>O3+Q3</f>
-        <v>17.61666666666666</v>
-      </c>
-      <c r="T3">
-        <f>O3+R3</f>
+        <f t="shared" si="3"/>
         <v>17.973333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <f>LOG10(C4)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C4">
@@ -8906,53 +7849,46 @@
         <v>18.88</v>
       </c>
       <c r="G4">
-        <v>0.66066666666666696</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H4">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="I4">
         <f>D4+G4</f>
-        <v>18.380666666666666</v>
-      </c>
-      <c r="J4">
-        <f>D4+H4</f>
         <v>18.849999999999998</v>
       </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>2.3010299956639813</v>
+      </c>
+      <c r="L4">
+        <v>200</v>
+      </c>
       <c r="M4">
-        <f>LOG10(N4)</f>
-        <v>2.3010299956639813</v>
+        <v>16.32</v>
       </c>
       <c r="N4">
-        <v>200</v>
+        <v>17.93</v>
       </c>
       <c r="O4">
-        <v>16.32</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P4">
-        <v>17.93</v>
+        <v>1.5533333333333299</v>
       </c>
       <c r="Q4">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>17.516666666666659</v>
       </c>
       <c r="R4">
-        <v>1.5533333333333299</v>
-      </c>
-      <c r="S4">
-        <f>O4+Q4</f>
-        <v>17.516666666666659</v>
-      </c>
-      <c r="T4">
-        <f>O4+R4</f>
+        <f t="shared" si="3"/>
         <v>17.873333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <f>LOG10(C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C5">
@@ -8968,53 +7904,46 @@
         <v>22.39</v>
       </c>
       <c r="G5">
-        <v>0.66066666666666696</v>
+        <v>0.97333333333333305</v>
       </c>
       <c r="H5">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="I5">
         <f>D5+G5</f>
-        <v>22.060666666666666</v>
-      </c>
-      <c r="J5">
-        <f>D5+H5</f>
-        <v>22.529999999999998</v>
+        <v>22.373333333333331</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="L5">
+        <v>20</v>
       </c>
       <c r="M5">
-        <f>LOG10(N5)</f>
-        <v>1.3010299956639813</v>
+        <v>19.95</v>
       </c>
       <c r="N5">
-        <v>20</v>
+        <v>21.46</v>
       </c>
       <c r="O5">
-        <v>19.95</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P5">
-        <v>21.46</v>
+        <v>1.57666666666666</v>
       </c>
       <c r="Q5">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>21.146666666666661</v>
       </c>
       <c r="R5">
-        <v>1.57666666666666</v>
-      </c>
-      <c r="S5">
-        <f>O5+Q5</f>
-        <v>21.146666666666661</v>
-      </c>
-      <c r="T5">
-        <f>O5+R5</f>
+        <f t="shared" si="3"/>
         <v>21.52666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <f>LOG10(C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C6">
@@ -9030,53 +7959,46 @@
         <v>22.43</v>
       </c>
       <c r="G6">
-        <v>0.66066666666666696</v>
+        <v>0.97333333333333305</v>
       </c>
       <c r="H6">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="I6">
         <f>D6+G6</f>
-        <v>22.230666666666668</v>
-      </c>
-      <c r="J6">
-        <f>D6+H6</f>
-        <v>22.7</v>
+        <v>22.543333333333333</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="L6">
+        <v>20</v>
       </c>
       <c r="M6">
-        <f>LOG10(N6)</f>
-        <v>1.3010299956639813</v>
+        <v>20.010000000000002</v>
       </c>
       <c r="N6">
-        <v>20</v>
+        <v>21.51</v>
       </c>
       <c r="O6">
-        <v>20.010000000000002</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P6">
-        <v>21.51</v>
+        <v>1.57666666666666</v>
       </c>
       <c r="Q6">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>21.206666666666663</v>
       </c>
       <c r="R6">
-        <v>1.57666666666666</v>
-      </c>
-      <c r="S6">
-        <f>O6+Q6</f>
-        <v>21.206666666666663</v>
-      </c>
-      <c r="T6">
-        <f>O6+R6</f>
+        <f t="shared" si="3"/>
         <v>21.586666666666662</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <f>LOG10(C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C7">
@@ -9092,53 +8014,46 @@
         <v>22.35</v>
       </c>
       <c r="G7">
-        <v>0.66066666666666696</v>
+        <v>0.97333333333333305</v>
       </c>
       <c r="H7">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="I7">
         <f>D7+G7</f>
-        <v>21.940666666666669</v>
-      </c>
-      <c r="J7">
-        <f>D7+H7</f>
-        <v>22.41</v>
+        <v>22.253333333333334</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="L7">
+        <v>20</v>
       </c>
       <c r="M7">
-        <f>LOG10(N7)</f>
-        <v>1.3010299956639813</v>
+        <v>19.850000000000001</v>
       </c>
       <c r="N7">
-        <v>20</v>
+        <v>21.6</v>
       </c>
       <c r="O7">
-        <v>19.850000000000001</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P7">
-        <v>21.6</v>
+        <v>1.57666666666666</v>
       </c>
       <c r="Q7">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>21.04666666666666</v>
       </c>
       <c r="R7">
-        <v>1.57666666666666</v>
-      </c>
-      <c r="S7">
-        <f>O7+Q7</f>
-        <v>21.04666666666666</v>
-      </c>
-      <c r="T7">
-        <f>O7+R7</f>
+        <f t="shared" si="3"/>
         <v>21.426666666666662</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
-        <f>LOG10(C8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C8">
@@ -9154,53 +8069,46 @@
         <v>25.44</v>
       </c>
       <c r="G8">
-        <v>0.66066666666666696</v>
+        <v>0.69333333333333302</v>
       </c>
       <c r="H8">
-        <v>1.0033333333333301</v>
-      </c>
-      <c r="I8">
         <f>D8+G8</f>
-        <v>25.520666666666667</v>
-      </c>
-      <c r="J8">
-        <f>D8+H8</f>
-        <v>25.86333333333333</v>
+        <v>25.553333333333331</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
       </c>
       <c r="M8">
-        <f>LOG10(N8)</f>
-        <v>0.3010299956639812</v>
+        <v>23.46</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>24.68</v>
       </c>
       <c r="O8">
-        <v>23.46</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P8">
-        <v>24.68</v>
+        <v>1.54</v>
       </c>
       <c r="Q8">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>24.656666666666659</v>
       </c>
       <c r="R8">
-        <v>1.54</v>
-      </c>
-      <c r="S8">
-        <f>O8+Q8</f>
-        <v>24.656666666666659</v>
-      </c>
-      <c r="T8">
-        <f>O8+R8</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
-        <f>LOG10(C9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9">
@@ -9216,53 +8124,46 @@
         <v>25.52</v>
       </c>
       <c r="G9">
-        <v>0.66066666666666696</v>
+        <v>0.69333333333333302</v>
       </c>
       <c r="H9">
-        <v>1.0033333333333301</v>
-      </c>
-      <c r="I9">
         <f>D9+G9</f>
-        <v>25.510666666666669</v>
-      </c>
-      <c r="J9">
-        <f>D9+H9</f>
-        <v>25.853333333333332</v>
+        <v>25.543333333333333</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
       </c>
       <c r="M9">
-        <f>LOG10(N9)</f>
-        <v>0.3010299956639812</v>
+        <v>23.51</v>
       </c>
       <c r="N9">
-        <v>2</v>
+        <v>24.66</v>
       </c>
       <c r="O9">
-        <v>23.51</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P9">
-        <v>24.66</v>
+        <v>1.54</v>
       </c>
       <c r="Q9">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>24.706666666666663</v>
       </c>
       <c r="R9">
-        <v>1.54</v>
-      </c>
-      <c r="S9">
-        <f>O9+Q9</f>
-        <v>24.706666666666663</v>
-      </c>
-      <c r="T9">
-        <f>O9+R9</f>
+        <f t="shared" si="3"/>
         <v>25.05</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
-        <f>LOG10(C10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C10">
@@ -9278,53 +8179,46 @@
         <v>25.53</v>
       </c>
       <c r="G10">
-        <v>0.66066666666666696</v>
+        <v>0.69333333333333302</v>
       </c>
       <c r="H10">
-        <v>1.0033333333333301</v>
-      </c>
-      <c r="I10">
         <f>D10+G10</f>
-        <v>25.360666666666667</v>
-      </c>
-      <c r="J10">
-        <f>D10+H10</f>
-        <v>25.70333333333333</v>
+        <v>25.393333333333331</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
       </c>
       <c r="M10">
-        <f>LOG10(N10)</f>
-        <v>0.3010299956639812</v>
+        <v>23.42</v>
       </c>
       <c r="N10">
-        <v>2</v>
+        <v>24.79</v>
       </c>
       <c r="O10">
-        <v>23.42</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P10">
-        <v>24.79</v>
+        <v>1.54</v>
       </c>
       <c r="Q10">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>24.61666666666666</v>
       </c>
       <c r="R10">
-        <v>1.54</v>
-      </c>
-      <c r="S10">
-        <f>O10+Q10</f>
-        <v>24.61666666666666</v>
-      </c>
-      <c r="T10">
-        <f>O10+R10</f>
+        <f t="shared" si="3"/>
         <v>24.96</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11">
-        <f>LOG10(C11)</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="C11">
@@ -9340,53 +8234,46 @@
         <v>28.34</v>
       </c>
       <c r="G11">
-        <v>0.66066666666666696</v>
+        <v>0.310000000000001</v>
       </c>
       <c r="H11">
-        <v>0.97333333333333305</v>
-      </c>
-      <c r="I11">
         <f>D11+G11</f>
-        <v>28.740666666666666</v>
-      </c>
-      <c r="J11">
-        <f>D11+H11</f>
-        <v>29.053333333333331</v>
+        <v>28.39</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>-0.69897000433601875</v>
+      </c>
+      <c r="L11">
+        <v>0.2</v>
       </c>
       <c r="M11">
-        <f>LOG10(N11)</f>
-        <v>-0.69897000433601875</v>
+        <v>26.61</v>
       </c>
       <c r="N11">
-        <v>0.2</v>
+        <v>27.62</v>
       </c>
       <c r="O11">
-        <v>26.61</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P11">
-        <v>27.62</v>
+        <v>1.58666666666666</v>
       </c>
       <c r="Q11">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>27.806666666666658</v>
       </c>
       <c r="R11">
-        <v>1.58666666666666</v>
-      </c>
-      <c r="S11">
-        <f>O11+Q11</f>
-        <v>27.806666666666658</v>
-      </c>
-      <c r="T11">
-        <f>O11+R11</f>
+        <f t="shared" si="3"/>
         <v>28.196666666666658</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12">
-        <f>LOG10(C12)</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="C12">
@@ -9402,53 +8289,46 @@
         <v>28.44</v>
       </c>
       <c r="G12">
-        <v>0.66066666666666696</v>
+        <v>0.310000000000001</v>
       </c>
       <c r="H12">
-        <v>0.97333333333333305</v>
-      </c>
-      <c r="I12">
         <f>D12+G12</f>
-        <v>28.750666666666667</v>
-      </c>
-      <c r="J12">
-        <f>D12+H12</f>
-        <v>29.063333333333333</v>
+        <v>28.400000000000002</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>-0.69897000433601875</v>
+      </c>
+      <c r="L12">
+        <v>0.2</v>
       </c>
       <c r="M12">
-        <f>LOG10(N12)</f>
-        <v>-0.69897000433601875</v>
+        <v>26.65</v>
       </c>
       <c r="N12">
-        <v>0.2</v>
+        <v>27.54</v>
       </c>
       <c r="O12">
-        <v>26.65</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P12">
-        <v>27.54</v>
+        <v>1.58666666666666</v>
       </c>
       <c r="Q12">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>27.846666666666657</v>
       </c>
       <c r="R12">
-        <v>1.58666666666666</v>
-      </c>
-      <c r="S12">
-        <f>O12+Q12</f>
-        <v>27.846666666666657</v>
-      </c>
-      <c r="T12">
-        <f>O12+R12</f>
+        <f t="shared" si="3"/>
         <v>28.236666666666657</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13">
-        <f>LOG10(C13)</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="C13">
@@ -9464,53 +8344,46 @@
         <v>28.32</v>
       </c>
       <c r="G13">
-        <v>0.66066666666666696</v>
+        <v>0.310000000000001</v>
       </c>
       <c r="H13">
-        <v>0.97333333333333305</v>
-      </c>
-      <c r="I13">
         <f>D13+G13</f>
-        <v>28.660666666666668</v>
-      </c>
-      <c r="J13">
-        <f>D13+H13</f>
-        <v>28.973333333333333</v>
+        <v>28.310000000000002</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>-0.69897000433601875</v>
+      </c>
+      <c r="L13">
+        <v>0.2</v>
       </c>
       <c r="M13">
-        <f>LOG10(N13)</f>
-        <v>-0.69897000433601875</v>
+        <v>26.53</v>
       </c>
       <c r="N13">
-        <v>0.2</v>
+        <v>27.62</v>
       </c>
       <c r="O13">
-        <v>26.53</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P13">
-        <v>27.62</v>
+        <v>1.58666666666666</v>
       </c>
       <c r="Q13">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>27.726666666666659</v>
       </c>
       <c r="R13">
-        <v>1.58666666666666</v>
-      </c>
-      <c r="S13">
-        <f>O13+Q13</f>
-        <v>27.726666666666659</v>
-      </c>
-      <c r="T13">
-        <f>O13+R13</f>
+        <f t="shared" si="3"/>
         <v>28.11666666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14">
-        <f>LOG10(C14)</f>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="C14">
@@ -9526,53 +8399,46 @@
         <v>31.18</v>
       </c>
       <c r="G14">
-        <v>0.66066666666666696</v>
+        <v>0.19666666666666599</v>
       </c>
       <c r="H14">
-        <v>0.836666666666667</v>
-      </c>
-      <c r="I14">
         <f>D14+G14</f>
-        <v>31.640666666666668</v>
-      </c>
-      <c r="J14">
-        <f>D14+H14</f>
-        <v>31.816666666666666</v>
+        <v>31.176666666666666</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>-1.6989700043360187</v>
+      </c>
+      <c r="L14">
+        <v>0.02</v>
       </c>
       <c r="M14">
-        <f>LOG10(N14)</f>
-        <v>-1.6989700043360187</v>
+        <v>29.6</v>
       </c>
       <c r="N14">
-        <v>0.02</v>
+        <v>30.14</v>
       </c>
       <c r="O14">
-        <v>29.6</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P14">
-        <v>30.14</v>
+        <v>1.48999999999999</v>
       </c>
       <c r="Q14">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>30.79666666666666</v>
       </c>
       <c r="R14">
-        <v>1.48999999999999</v>
-      </c>
-      <c r="S14">
-        <f>O14+Q14</f>
-        <v>30.79666666666666</v>
-      </c>
-      <c r="T14">
-        <f>O14+R14</f>
+        <f t="shared" si="3"/>
         <v>31.089999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15">
-        <f>LOG10(C15)</f>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="C15">
@@ -9588,53 +8454,46 @@
         <v>31.18</v>
       </c>
       <c r="G15">
-        <v>0.66066666666666696</v>
+        <v>0.19666666666666599</v>
       </c>
       <c r="H15">
-        <v>0.836666666666667</v>
-      </c>
-      <c r="I15">
         <f>D15+G15</f>
-        <v>31.610666666666667</v>
-      </c>
-      <c r="J15">
-        <f>D15+H15</f>
-        <v>31.786666666666665</v>
+        <v>31.146666666666665</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>-1.6989700043360187</v>
+      </c>
+      <c r="L15">
+        <v>0.02</v>
       </c>
       <c r="M15">
-        <f>LOG10(N15)</f>
-        <v>-1.6989700043360187</v>
+        <v>29.61</v>
       </c>
       <c r="N15">
-        <v>0.02</v>
+        <v>30.18</v>
       </c>
       <c r="O15">
-        <v>29.61</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P15">
-        <v>30.18</v>
+        <v>1.48999999999999</v>
       </c>
       <c r="Q15">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>30.806666666666658</v>
       </c>
       <c r="R15">
-        <v>1.48999999999999</v>
-      </c>
-      <c r="S15">
-        <f>O15+Q15</f>
-        <v>30.806666666666658</v>
-      </c>
-      <c r="T15">
-        <f>O15+R15</f>
+        <f t="shared" si="3"/>
         <v>31.099999999999991</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16">
-        <f>LOG10(C16)</f>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="C16">
@@ -9650,44 +8509,37 @@
         <v>31.13</v>
       </c>
       <c r="G16">
-        <v>0.66066666666666696</v>
+        <v>0.19666666666666599</v>
       </c>
       <c r="H16">
-        <v>0.836666666666667</v>
-      </c>
-      <c r="I16">
         <f>D16+G16</f>
-        <v>31.630666666666666</v>
-      </c>
-      <c r="J16">
-        <f>D16+H16</f>
-        <v>31.806666666666665</v>
+        <v>31.166666666666664</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>-1.6989700043360187</v>
+      </c>
+      <c r="L16">
+        <v>0.02</v>
       </c>
       <c r="M16">
-        <f>LOG10(N16)</f>
-        <v>-1.6989700043360187</v>
+        <v>29.44</v>
       </c>
       <c r="N16">
-        <v>0.02</v>
+        <v>30.13</v>
       </c>
       <c r="O16">
-        <v>29.44</v>
+        <v>1.1966666666666601</v>
       </c>
       <c r="P16">
-        <v>30.13</v>
+        <v>1.48999999999999</v>
       </c>
       <c r="Q16">
-        <v>1.1966666666666601</v>
+        <f t="shared" si="2"/>
+        <v>30.636666666666663</v>
       </c>
       <c r="R16">
-        <v>1.48999999999999</v>
-      </c>
-      <c r="S16">
-        <f>O16+Q16</f>
-        <v>30.636666666666663</v>
-      </c>
-      <c r="T16">
-        <f>O16+R16</f>
+        <f t="shared" si="3"/>
         <v>30.929999999999993</v>
       </c>
     </row>

</xml_diff>